<commit_message>
Add GUI for feedback form generation
Implemented a Tkinter-based GUI for creating student feedback forms from Excel files. This includes features for selecting Excel/Word files, updating configuration settings, and generating feedback forms with optional rubric inclusion.
</commit_message>
<xml_diff>
--- a/Example_Marks.xlsx
+++ b/Example_Marks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\AutoFeedback\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\FeedbackCreator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C206F3A-6494-4FE7-812F-E6D400A27219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE03E270-87B7-456A-A5EC-0212DE1E87D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7010" yWindow="5260" windowWidth="28800" windowHeight="15410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="28800" windowHeight="15410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,45 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Ure, Alper</t>
-  </si>
-  <si>
-    <t>Hi Lewis,
-I've reviewed your submission and noticed that it includes only the turntable video of the skull element, which lacks some of the necessary anatomical details and precision expected. The character blockout is also missing. I've also observed that you have not been able to attend any of the classes where we discussed these critical components. Attendance is important as it helps you understand the foundational skills and the detailed requirements of your projects. Please make an effort to catch up on what you've missed and ensure all required elements are included in your future submissions. If there are any obstacles you're facing regarding attendance or the coursework, please don't hesitate to reach out for assistance.</t>
-  </si>
-  <si>
-    <t>Hi Lauren,
-Great job on your presentation! It was exceptionally clear and well-structured—so much so that I could certainly use it as a model for how to present work effectively. Your skeleton sculpture also stood out, particularly for its tangible, clay-like quality that brings a lot of character to the piece.
-You did an excellent job sculpting the hands and feet; the attention to detail in these areas is commendable and they are well-executed with a high level of craftsmanship. These elements add a professional touch to your overall creation, enhancing the sculpture's realism.
-However, there are a few anatomical adjustments that could further improve its accuracy. The spine, for instance, appears a bit misshaped at the top, with the segments showing an unusual triangular protrusion at the front. Introducing slight gaps between these segments could make the spine look more lifelike. Additionally, while the wobbly legs add a unique touch, they detract from the anatomical accuracy. Addressing these points will refine your sculpture and elevate the quality of your work.
-Keep up the great work, Lauren! Your ability to capture such intricate details is impressive, and with a few tweaks, your sculpture could reach an even higher standard of excellence. If you need any resources or further clarification, please don’t hesitate to reach out.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Hi Alper,
-Your presentation was outstanding—thorough and richly detailed, it effectively conveyed your deep understanding of the assignment.
-The bone shapes in your work were particularly well-executed, showcasing your ability to create forms that are both accurate and aesthetically pleasing. The level of detail in your presentation was commendable, and it's clear that you've put a lot of thought and effort into every aspect of your project.
-There was a slight issue with playing the turnaround video, but the detailed visuals you provided in your presentation compensated well for this hiccup. It’s hard to find any faults given the high quality of your submission.
-Overall, you’ve done an excellent job. Keep up the great work, and continue to apply the same meticulous attention to detail in your future projects. If you need any assistance with the technical aspects or any other part of your coursework, please don’t hesitate to reach out.</t>
-  </si>
-  <si>
-    <t>Hi Anastasia,
-I really appreciated your choice to focus on a frog study for this project. The final model you presented turned out well and showcases your skillful approach to sculpting. There were a few bumpy areas on the hip element that you might want to smooth out for a cleaner look in future projects.
-Your presentation was delivered clearly and confidently, which made it easy to follow along and understand your process and decisions. The turn-around of your model was particularly interesting; it highlighted the importance of showing the bottom of the base, a detail often overlooked but clearly significant as demonstrated by your work.
-Overall, you've done a commendable job on this assignment. Keep up the great work and continue to refine your techniques to enhance your sculpting even further. If you need any resources or further guidance, please feel free to reach out.</t>
-  </si>
-  <si>
-    <t>Hi Thomas,
-It’s really unfortunate that you lost your work due to hard drive issues, but I'm impressed with how well the end result turned out despite this setback. The skull, hands, and feet are particularly well done. The chunkiness you've given the feet adds a sense of boldness and confidence to your sculpting style, which is very appealing. The silver shader you chose also adds a nice touch, enhancing the overall visual impact of your piece.
-The headless turnaround was effective, and I understand the practical reasons for the missing skull in this rendition. However, the ribs seem a bit too pronounced, projecting outward more than is typical. Scaling these back slightly could improve the anatomical accuracy and give a more natural look to the torso.
-Overall, you’ve done a commendable job. Focusing on refining the ribcage, especially the front of the ribs, will help elevate your sculpture even further. Keep up the great work, and I look forward to seeing how you apply these improvements in future projects. If you need any assistance or further feedback, feel free to reach out.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mark </t>
   </si>
   <si>
@@ -76,22 +42,7 @@
     <t>Crick, Jo</t>
   </si>
   <si>
-    <t>Owens, Mike</t>
-  </si>
-  <si>
-    <t>Shirley, Poop</t>
-  </si>
-  <si>
-    <t>Iqbal, Jackie</t>
-  </si>
-  <si>
-    <t>great</t>
-  </si>
-  <si>
-    <t>James, Dean</t>
-  </si>
-  <si>
-    <t>Moving forward, keep focusing on the accuracy of all anatomical elements as you have with the hands and feet. Great job persevering through the technical difficulties, and I look forward to seeing how you apply these learnings to future projects. If you need help with data backup strategies or any other assistance, please don’t hesitate to ask.</t>
+    <t>Example Feedback</t>
   </si>
 </sst>
 </file>
@@ -457,7 +408,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -473,90 +424,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D1"/>
     </row>
     <row r="2" spans="1:4" ht="42" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>53</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>54</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>65</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <v>44</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>56</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7">
-        <v>76</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8">
-        <v>44</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
+    <row r="4" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:4" ht="53.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>